<commit_message>
external postgres DB is implemented button component is modified
</commit_message>
<xml_diff>
--- a/back-end/SettingsCMS.xlsx
+++ b/back-end/SettingsCMS.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="B1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,30 +442,27 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>projectName</t>
+          <t>cmsName</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>backgroundColor</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Super Market</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>#c0ffee</t>
+          <t>cmsBackgroundColor</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>titleBackgroundColor</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>titleTextColor</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>cardBackgroundColor</t>
         </is>
       </c>
     </row>

</xml_diff>